<commit_message>
Update-Delete of Sumfone Tagadad
</commit_message>
<xml_diff>
--- a/DataIn/VarExpl/20_RevVar.Expl_RedConflitGeralTot.xlsx
+++ b/DataIn/VarExpl/20_RevVar.Expl_RedConflitGeralTot.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a6b088a06617d4fb/Ejercicio 7/Documents/Documents/Maestria/Modelado_Merlin/GitHub_Datos/Social_Model_Enchugal/DataIn/VarExpl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{BDDC5DEC-868D-42DE-AD1A-BC98CB238E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31ACD3DC-4CEC-4276-A524-C213787338C6}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{BDDC5DEC-868D-42DE-AD1A-BC98CB238E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3AF42E2F-B648-4092-A277-C716DBA789D8}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="3" xr2:uid="{9786ED26-BEA9-40A5-9EEA-8A67307F5FD0}"/>
+    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="3" xr2:uid="{9786ED26-BEA9-40A5-9EEA-8A67307F5FD0}"/>
   </bookViews>
   <sheets>
     <sheet name="RedeConflitGerTotal_List" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="247">
   <si>
     <t xml:space="preserve">Antonio Mbunh </t>
   </si>
@@ -865,6 +865,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
@@ -55222,10 +55226,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE5DEE8A-743F-487A-BABB-5CF40CDB2794}">
-  <dimension ref="A1:Q131"/>
+  <dimension ref="A1:Q130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="R19" sqref="R19"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="I82" sqref="I82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -59369,7 +59373,7 @@
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B79">
         <v>0</v>
@@ -59422,7 +59426,7 @@
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>183</v>
+        <v>79</v>
       </c>
       <c r="B80">
         <v>0</v>
@@ -59475,7 +59479,7 @@
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B81">
         <v>0</v>
@@ -59528,7 +59532,7 @@
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B82">
         <v>0</v>
@@ -59581,7 +59585,7 @@
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B83">
         <v>0</v>
@@ -59634,7 +59638,7 @@
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B84">
         <v>0</v>
@@ -59687,7 +59691,7 @@
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>83</v>
+        <v>184</v>
       </c>
       <c r="B85">
         <v>0</v>
@@ -59740,43 +59744,43 @@
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>184</v>
+        <v>85</v>
       </c>
       <c r="B86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F86">
-        <v>0</v>
+        <v>3.0221456661820401E-2</v>
       </c>
       <c r="G86">
-        <v>0</v>
+        <v>2.86187436431646E-2</v>
       </c>
       <c r="H86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L86">
-        <v>903</v>
+        <v>897</v>
       </c>
       <c r="M86">
-        <v>903</v>
+        <v>897</v>
       </c>
       <c r="N86">
         <v>0</v>
@@ -59784,52 +59788,52 @@
       <c r="O86">
         <v>0</v>
       </c>
-      <c r="P86">
-        <v>-1.2485092156566701E-4</v>
+      <c r="P86" s="7">
+        <v>-3.7268932828737901E-6</v>
       </c>
       <c r="Q86" s="7">
-        <v>-7.5112424383405596E-5</v>
+        <v>4.6011602535145398E-5</v>
       </c>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F87">
-        <v>3.0221456661820401E-2</v>
+        <v>0</v>
       </c>
       <c r="G87">
-        <v>2.86187436431646E-2</v>
+        <v>0</v>
       </c>
       <c r="H87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L87">
-        <v>897</v>
+        <v>903</v>
       </c>
       <c r="M87">
-        <v>897</v>
+        <v>903</v>
       </c>
       <c r="N87">
         <v>0</v>
@@ -59837,16 +59841,16 @@
       <c r="O87">
         <v>0</v>
       </c>
-      <c r="P87" s="7">
-        <v>-3.7268932828737901E-6</v>
+      <c r="P87">
+        <v>-1.2485092156566701E-4</v>
       </c>
       <c r="Q87" s="7">
-        <v>4.6011602535145398E-5</v>
+        <v>-7.5112424383405596E-5</v>
       </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>86</v>
+        <v>185</v>
       </c>
       <c r="B88">
         <v>0</v>
@@ -59899,113 +59903,113 @@
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>185</v>
+        <v>139</v>
       </c>
       <c r="B89">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C89">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D89">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E89">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F89">
-        <v>0</v>
+        <v>17.5084838867187</v>
       </c>
       <c r="G89">
-        <v>0</v>
+        <v>5.5883684158325204</v>
       </c>
       <c r="H89">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I89">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J89">
-        <v>0</v>
+        <v>3.7833333015441899</v>
       </c>
       <c r="K89">
-        <v>0</v>
+        <v>4.1999998092651403</v>
       </c>
       <c r="L89">
-        <v>903</v>
+        <v>867</v>
       </c>
       <c r="M89">
-        <v>903</v>
+        <v>867</v>
       </c>
       <c r="N89">
-        <v>0</v>
+        <v>12.6666669845581</v>
       </c>
       <c r="O89">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P89">
-        <v>-1.2485092156566701E-4</v>
-      </c>
-      <c r="Q89" s="7">
-        <v>-7.5112424383405596E-5</v>
+        <v>1.5708855353295801E-3</v>
+      </c>
+      <c r="Q89">
+        <v>5.84004155825823E-4</v>
       </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>139</v>
+        <v>186</v>
       </c>
       <c r="B90">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C90">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D90">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E90">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F90">
-        <v>17.5084838867187</v>
+        <v>0</v>
       </c>
       <c r="G90">
-        <v>5.5883684158325204</v>
+        <v>0</v>
       </c>
       <c r="H90">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I90">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J90">
-        <v>3.7833333015441899</v>
+        <v>0</v>
       </c>
       <c r="K90">
-        <v>4.1999998092651403</v>
+        <v>0</v>
       </c>
       <c r="L90">
-        <v>867</v>
+        <v>903</v>
       </c>
       <c r="M90">
-        <v>867</v>
+        <v>903</v>
       </c>
       <c r="N90">
-        <v>12.6666669845581</v>
+        <v>0</v>
       </c>
       <c r="O90">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P90">
-        <v>1.5708855353295801E-3</v>
-      </c>
-      <c r="Q90">
-        <v>5.84004155825823E-4</v>
+        <v>-1.2485092156566701E-4</v>
+      </c>
+      <c r="Q90" s="7">
+        <v>-7.5112424383405596E-5</v>
       </c>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>186</v>
+        <v>90</v>
       </c>
       <c r="B91">
         <v>0</v>
@@ -60058,7 +60062,7 @@
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>90</v>
+        <v>187</v>
       </c>
       <c r="B92">
         <v>0</v>
@@ -60111,43 +60115,43 @@
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>187</v>
+        <v>152</v>
       </c>
       <c r="B93">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C93">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D93">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E93">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F93">
-        <v>0</v>
+        <v>30.181612014770501</v>
       </c>
       <c r="G93">
-        <v>0</v>
+        <v>30.274787902831999</v>
       </c>
       <c r="H93">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I93">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J93">
-        <v>0</v>
+        <v>4.1666665077209499</v>
       </c>
       <c r="K93">
-        <v>0</v>
+        <v>4.3666667938232404</v>
       </c>
       <c r="L93">
-        <v>903</v>
+        <v>863</v>
       </c>
       <c r="M93">
-        <v>903</v>
+        <v>861</v>
       </c>
       <c r="N93">
         <v>0</v>
@@ -60156,51 +60160,51 @@
         <v>0</v>
       </c>
       <c r="P93">
-        <v>-1.2485092156566701E-4</v>
-      </c>
-      <c r="Q93" s="7">
-        <v>-7.5112424383405596E-5</v>
+        <v>1.02582736872137E-3</v>
+      </c>
+      <c r="Q93">
+        <v>4.4168342719785902E-4</v>
       </c>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>152</v>
+        <v>188</v>
       </c>
       <c r="B94">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C94">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D94">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E94">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F94">
-        <v>30.181612014770501</v>
+        <v>0</v>
       </c>
       <c r="G94">
-        <v>30.274787902831999</v>
+        <v>0</v>
       </c>
       <c r="H94">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I94">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J94">
-        <v>4.1666665077209499</v>
+        <v>0</v>
       </c>
       <c r="K94">
-        <v>4.3666667938232404</v>
+        <v>0</v>
       </c>
       <c r="L94">
-        <v>863</v>
+        <v>903</v>
       </c>
       <c r="M94">
-        <v>861</v>
+        <v>903</v>
       </c>
       <c r="N94">
         <v>0</v>
@@ -60209,15 +60213,15 @@
         <v>0</v>
       </c>
       <c r="P94">
-        <v>1.02582736872137E-3</v>
-      </c>
-      <c r="Q94">
-        <v>4.4168342719785902E-4</v>
+        <v>-1.2485092156566701E-4</v>
+      </c>
+      <c r="Q94" s="7">
+        <v>-7.5112424383405596E-5</v>
       </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>188</v>
+        <v>94</v>
       </c>
       <c r="B95">
         <v>0</v>
@@ -60270,7 +60274,7 @@
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B96">
         <v>0</v>
@@ -60323,43 +60327,43 @@
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>95</v>
+        <v>133</v>
       </c>
       <c r="B97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F97">
-        <v>0</v>
+        <v>3.0221456661820401E-2</v>
       </c>
       <c r="G97">
-        <v>0</v>
+        <v>2.86187436431646E-2</v>
       </c>
       <c r="H97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L97">
-        <v>903</v>
+        <v>897</v>
       </c>
       <c r="M97">
-        <v>903</v>
+        <v>897</v>
       </c>
       <c r="N97">
         <v>0</v>
@@ -60367,52 +60371,52 @@
       <c r="O97">
         <v>0</v>
       </c>
-      <c r="P97">
-        <v>-1.2485092156566701E-4</v>
+      <c r="P97" s="7">
+        <v>-3.7268932828737901E-6</v>
       </c>
       <c r="Q97" s="7">
-        <v>-7.5112424383405596E-5</v>
+        <v>4.6011602535145398E-5</v>
       </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>133</v>
+        <v>97</v>
       </c>
       <c r="B98">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C98">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D98">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E98">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F98">
-        <v>3.0221456661820401E-2</v>
+        <v>0</v>
       </c>
       <c r="G98">
-        <v>2.86187436431646E-2</v>
+        <v>0</v>
       </c>
       <c r="H98">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I98">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J98">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K98">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L98">
-        <v>897</v>
+        <v>903</v>
       </c>
       <c r="M98">
-        <v>897</v>
+        <v>903</v>
       </c>
       <c r="N98">
         <v>0</v>
@@ -60420,52 +60424,52 @@
       <c r="O98">
         <v>0</v>
       </c>
-      <c r="P98" s="7">
-        <v>-3.7268932828737901E-6</v>
+      <c r="P98">
+        <v>-1.2485092156566701E-4</v>
       </c>
       <c r="Q98" s="7">
-        <v>4.6011602535145398E-5</v>
+        <v>-7.5112424383405596E-5</v>
       </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>97</v>
+        <v>137</v>
       </c>
       <c r="B99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F99">
-        <v>0</v>
+        <v>3.0221456661820401E-2</v>
       </c>
       <c r="G99">
-        <v>0</v>
+        <v>2.86187436431646E-2</v>
       </c>
       <c r="H99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L99">
-        <v>903</v>
+        <v>897</v>
       </c>
       <c r="M99">
-        <v>903</v>
+        <v>897</v>
       </c>
       <c r="N99">
         <v>0</v>
@@ -60473,52 +60477,52 @@
       <c r="O99">
         <v>0</v>
       </c>
-      <c r="P99">
-        <v>-1.2485092156566701E-4</v>
+      <c r="P99" s="7">
+        <v>-3.7268932828737901E-6</v>
       </c>
       <c r="Q99" s="7">
-        <v>-7.5112424383405596E-5</v>
+        <v>4.6011602535145398E-5</v>
       </c>
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>137</v>
+        <v>99</v>
       </c>
       <c r="B100">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C100">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D100">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E100">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F100">
-        <v>3.0221456661820401E-2</v>
+        <v>0</v>
       </c>
       <c r="G100">
-        <v>2.86187436431646E-2</v>
+        <v>0</v>
       </c>
       <c r="H100">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I100">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J100">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K100">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L100">
-        <v>897</v>
+        <v>903</v>
       </c>
       <c r="M100">
-        <v>897</v>
+        <v>903</v>
       </c>
       <c r="N100">
         <v>0</v>
@@ -60526,52 +60530,52 @@
       <c r="O100">
         <v>0</v>
       </c>
-      <c r="P100" s="7">
-        <v>-3.7268932828737901E-6</v>
+      <c r="P100">
+        <v>-1.2485092156566701E-4</v>
       </c>
       <c r="Q100" s="7">
-        <v>4.6011602535145398E-5</v>
+        <v>-7.5112424383405596E-5</v>
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B101">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C101">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D101">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E101">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F101">
-        <v>0</v>
+        <v>3.0221456661820401E-2</v>
       </c>
       <c r="G101">
-        <v>0</v>
+        <v>2.86187436431646E-2</v>
       </c>
       <c r="H101">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I101">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J101">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K101">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L101">
-        <v>903</v>
+        <v>897</v>
       </c>
       <c r="M101">
-        <v>903</v>
+        <v>897</v>
       </c>
       <c r="N101">
         <v>0</v>
@@ -60579,52 +60583,52 @@
       <c r="O101">
         <v>0</v>
       </c>
-      <c r="P101">
-        <v>-1.2485092156566701E-4</v>
+      <c r="P101" s="7">
+        <v>-3.7268932828737901E-6</v>
       </c>
       <c r="Q101" s="7">
-        <v>-7.5112424383405596E-5</v>
+        <v>4.6011602535145398E-5</v>
       </c>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B102">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C102">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D102">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E102">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F102">
-        <v>3.0221456661820401E-2</v>
+        <v>0</v>
       </c>
       <c r="G102">
-        <v>2.86187436431646E-2</v>
+        <v>0</v>
       </c>
       <c r="H102">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I102">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J102">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K102">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L102">
-        <v>897</v>
+        <v>903</v>
       </c>
       <c r="M102">
-        <v>897</v>
+        <v>903</v>
       </c>
       <c r="N102">
         <v>0</v>
@@ -60632,16 +60636,16 @@
       <c r="O102">
         <v>0</v>
       </c>
-      <c r="P102" s="7">
-        <v>-3.7268932828737901E-6</v>
+      <c r="P102">
+        <v>-1.2485092156566701E-4</v>
       </c>
       <c r="Q102" s="7">
-        <v>4.6011602535145398E-5</v>
+        <v>-7.5112424383405596E-5</v>
       </c>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B103">
         <v>0</v>
@@ -60694,7 +60698,7 @@
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B104">
         <v>0</v>
@@ -60747,7 +60751,7 @@
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B105">
         <v>0</v>
@@ -60800,7 +60804,7 @@
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B106">
         <v>0</v>
@@ -60853,7 +60857,7 @@
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B107">
         <v>0</v>
@@ -60906,43 +60910,43 @@
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B108">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C108">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D108">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E108">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F108">
-        <v>0</v>
+        <v>4.7437891364097602E-2</v>
       </c>
       <c r="G108">
-        <v>0</v>
+        <v>4.4922154396772399E-2</v>
       </c>
       <c r="H108">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I108">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J108">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="K108">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="L108">
-        <v>903</v>
+        <v>892</v>
       </c>
       <c r="M108">
-        <v>903</v>
+        <v>892</v>
       </c>
       <c r="N108">
         <v>0</v>
@@ -60951,51 +60955,51 @@
         <v>0</v>
       </c>
       <c r="P108">
-        <v>-1.2485092156566701E-4</v>
-      </c>
-      <c r="Q108" s="7">
-        <v>-7.5112424383405596E-5</v>
+        <v>1.17397139547393E-4</v>
+      </c>
+      <c r="Q108">
+        <v>1.06573621451389E-4</v>
       </c>
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>107</v>
+        <v>189</v>
       </c>
       <c r="B109">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C109">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D109">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E109">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F109">
-        <v>4.7437891364097602E-2</v>
+        <v>0</v>
       </c>
       <c r="G109">
-        <v>4.4922154396772399E-2</v>
+        <v>0</v>
       </c>
       <c r="H109">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I109">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J109">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="K109">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="L109">
-        <v>892</v>
+        <v>903</v>
       </c>
       <c r="M109">
-        <v>892</v>
+        <v>903</v>
       </c>
       <c r="N109">
         <v>0</v>
@@ -61004,15 +61008,15 @@
         <v>0</v>
       </c>
       <c r="P109">
-        <v>1.17397139547393E-4</v>
-      </c>
-      <c r="Q109">
-        <v>1.06573621451389E-4</v>
+        <v>-1.2485092156566701E-4</v>
+      </c>
+      <c r="Q109" s="7">
+        <v>-7.5112424383405596E-5</v>
       </c>
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B110">
         <v>0</v>
@@ -61065,7 +61069,7 @@
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>190</v>
+        <v>110</v>
       </c>
       <c r="B111">
         <v>0</v>
@@ -61118,7 +61122,7 @@
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>110</v>
+        <v>191</v>
       </c>
       <c r="B112">
         <v>0</v>
@@ -61171,7 +61175,7 @@
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B113">
         <v>0</v>
@@ -61224,7 +61228,7 @@
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>192</v>
+        <v>113</v>
       </c>
       <c r="B114">
         <v>0</v>
@@ -61277,43 +61281,43 @@
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>113</v>
+        <v>193</v>
       </c>
       <c r="B115">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C115">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D115">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E115">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F115">
-        <v>0</v>
+        <v>3.0221456661820401E-2</v>
       </c>
       <c r="G115">
-        <v>0</v>
+        <v>2.86187436431646E-2</v>
       </c>
       <c r="H115">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I115">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J115">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K115">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L115">
-        <v>903</v>
+        <v>897</v>
       </c>
       <c r="M115">
-        <v>903</v>
+        <v>897</v>
       </c>
       <c r="N115">
         <v>0</v>
@@ -61321,52 +61325,52 @@
       <c r="O115">
         <v>0</v>
       </c>
-      <c r="P115">
-        <v>-1.2485092156566701E-4</v>
+      <c r="P115" s="7">
+        <v>-3.7268932828737901E-6</v>
       </c>
       <c r="Q115" s="7">
-        <v>-7.5112424383405596E-5</v>
+        <v>4.6011602535145398E-5</v>
       </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>193</v>
+        <v>115</v>
       </c>
       <c r="B116">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C116">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D116">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E116">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F116">
-        <v>3.0221456661820401E-2</v>
+        <v>0</v>
       </c>
       <c r="G116">
-        <v>2.86187436431646E-2</v>
+        <v>0</v>
       </c>
       <c r="H116">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I116">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J116">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K116">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L116">
-        <v>897</v>
+        <v>903</v>
       </c>
       <c r="M116">
-        <v>897</v>
+        <v>903</v>
       </c>
       <c r="N116">
         <v>0</v>
@@ -61374,16 +61378,16 @@
       <c r="O116">
         <v>0</v>
       </c>
-      <c r="P116" s="7">
-        <v>-3.7268932828737901E-6</v>
+      <c r="P116">
+        <v>-1.2485092156566701E-4</v>
       </c>
       <c r="Q116" s="7">
-        <v>4.6011602535145398E-5</v>
+        <v>-7.5112424383405596E-5</v>
       </c>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B117">
         <v>0</v>
@@ -61436,7 +61440,7 @@
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>116</v>
+        <v>194</v>
       </c>
       <c r="B118">
         <v>0</v>
@@ -61489,7 +61493,7 @@
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B119">
         <v>0</v>
@@ -61542,7 +61546,7 @@
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B120">
         <v>0</v>
@@ -61595,7 +61599,7 @@
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>196</v>
+        <v>120</v>
       </c>
       <c r="B121">
         <v>0</v>
@@ -61648,7 +61652,7 @@
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B122">
         <v>0</v>
@@ -61701,7 +61705,7 @@
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>121</v>
+        <v>197</v>
       </c>
       <c r="B123">
         <v>0</v>
@@ -61754,7 +61758,7 @@
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B124">
         <v>0</v>
@@ -61807,7 +61811,7 @@
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B125">
         <v>0</v>
@@ -61860,7 +61864,7 @@
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>199</v>
+        <v>125</v>
       </c>
       <c r="B126">
         <v>0</v>
@@ -61913,7 +61917,7 @@
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B127">
         <v>0</v>
@@ -61966,7 +61970,7 @@
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B128">
         <v>0</v>
@@ -62019,7 +62023,7 @@
     </row>
     <row r="129" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B129">
         <v>0</v>
@@ -62072,7 +62076,7 @@
     </row>
     <row r="130" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B130">
         <v>0</v>
@@ -62120,59 +62124,6 @@
         <v>-1.2485092156566701E-4</v>
       </c>
       <c r="Q130" s="7">
-        <v>-7.5112424383405596E-5</v>
-      </c>
-    </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A131" t="s">
-        <v>129</v>
-      </c>
-      <c r="B131">
-        <v>0</v>
-      </c>
-      <c r="C131">
-        <v>0</v>
-      </c>
-      <c r="D131">
-        <v>0</v>
-      </c>
-      <c r="E131">
-        <v>0</v>
-      </c>
-      <c r="F131">
-        <v>0</v>
-      </c>
-      <c r="G131">
-        <v>0</v>
-      </c>
-      <c r="H131">
-        <v>0</v>
-      </c>
-      <c r="I131">
-        <v>0</v>
-      </c>
-      <c r="J131">
-        <v>0</v>
-      </c>
-      <c r="K131">
-        <v>0</v>
-      </c>
-      <c r="L131">
-        <v>903</v>
-      </c>
-      <c r="M131">
-        <v>903</v>
-      </c>
-      <c r="N131">
-        <v>0</v>
-      </c>
-      <c r="O131">
-        <v>0</v>
-      </c>
-      <c r="P131">
-        <v>-1.2485092156566701E-4</v>
-      </c>
-      <c r="Q131" s="7">
         <v>-7.5112424383405596E-5</v>
       </c>
     </row>

</xml_diff>